<commit_message>
objective 1C: requirements, design, half implementation
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A11AE38-5C14-4373-AAF7-8A3B2956E044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2D3AE-E7C6-464B-89D5-F4B2591BC0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2090" yWindow="30" windowWidth="19640" windowHeight="20480" activeTab="1" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="3530" yWindow="140" windowWidth="19640" windowHeight="20480" activeTab="1" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -352,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -445,15 +445,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1629,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9F7A41-D1C8-40CA-B4D4-A4E7F54E7CAD}">
   <dimension ref="A1:BN56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2306,6 +2307,7 @@
       <c r="Z12" s="25"/>
       <c r="AA12" s="26"/>
       <c r="AB12" s="27"/>
+      <c r="AN12" s="28"/>
     </row>
     <row r="13" spans="1:66" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -2321,6 +2323,9 @@
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="27"/>
+      <c r="AC13" s="55"/>
+      <c r="AD13" s="55"/>
+      <c r="AE13" s="55"/>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>

</xml_diff>

<commit_message>
added guard search ish and gitignore
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367B7672-D9AB-4870-A8ED-A564612C9EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE714FFC-982F-4AF0-BBD2-18AE98706282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -885,7 +885,7 @@
   <dimension ref="A1:DY57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CE14" sqref="CE14"/>
+      <selection activeCell="BH12" sqref="BH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2142,7 +2142,7 @@
       <c r="K12" s="44"/>
       <c r="AN12" s="46"/>
       <c r="AX12" s="57"/>
-      <c r="AY12" s="28"/>
+      <c r="AY12" s="9"/>
       <c r="AZ12" s="29"/>
     </row>
     <row r="13" spans="1:129" ht="58" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
broken group search, 4 guards all search together
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE714FFC-982F-4AF0-BBD2-18AE98706282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D866BFB-C585-4789-9FC2-1AC708A31CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="3530" yWindow="140" windowWidth="19640" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -885,7 +885,7 @@
   <dimension ref="A1:DY57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BH12" sqref="BH12"/>
+      <selection activeCell="BB13" sqref="BB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2143,7 +2143,7 @@
       <c r="AN12" s="46"/>
       <c r="AX12" s="57"/>
       <c r="AY12" s="9"/>
-      <c r="AZ12" s="29"/>
+      <c r="AZ12" s="10"/>
     </row>
     <row r="13" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
fixed group guard search, broken guard patrol paths
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D866BFB-C585-4789-9FC2-1AC708A31CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC22B25-B475-433C-B31E-690EBD0B4EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3530" yWindow="140" windowWidth="19640" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -885,7 +885,7 @@
   <dimension ref="A1:DY57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BB13" sqref="BB13"/>
+      <selection activeCell="BW14" sqref="BW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2144,6 +2144,7 @@
       <c r="AX12" s="57"/>
       <c r="AY12" s="9"/>
       <c r="AZ12" s="10"/>
+      <c r="BA12" s="23"/>
     </row>
     <row r="13" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
guard patrol paths fixed. documentation still to do.
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC22B25-B475-433C-B31E-690EBD0B4EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDDF7FB-28B1-4006-9058-333F4EB72DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -885,7 +885,7 @@
   <dimension ref="A1:DY57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BW14" sqref="BW14"/>
+      <selection activeCell="BF12" sqref="BF12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2145,6 +2145,9 @@
       <c r="AY12" s="9"/>
       <c r="AZ12" s="10"/>
       <c r="BA12" s="23"/>
+      <c r="BB12" s="23"/>
+      <c r="BC12" s="23"/>
+      <c r="BD12" s="23"/>
     </row>
     <row r="13" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
Objective 1B completed, write-up completed up to now
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDDF7FB-28B1-4006-9058-333F4EB72DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9F5BE2-3CAB-4128-AAD7-B054A642B629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -339,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -447,11 +447,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -568,6 +588,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,7 +910,7 @@
   <dimension ref="A1:DY57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BF12" sqref="BF12"/>
+      <selection activeCell="BR13" sqref="BR13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2110,7 +2135,7 @@
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="J11" s="42"/>
@@ -2119,10 +2144,10 @@
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
       <c r="O11" s="44"/>
-      <c r="AZ11" s="27"/>
-      <c r="BA11" s="28"/>
-      <c r="BB11" s="28"/>
-      <c r="BC11" s="29"/>
+      <c r="AZ11" s="58"/>
+      <c r="BA11" s="59"/>
+      <c r="BB11" s="59"/>
+      <c r="BC11" s="60"/>
     </row>
     <row r="12" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -2131,11 +2156,13 @@
       <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="56">
         <v>45020</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="56">
+        <v>45038</v>
+      </c>
       <c r="H12" s="42"/>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
@@ -2143,11 +2170,12 @@
       <c r="AN12" s="46"/>
       <c r="AX12" s="57"/>
       <c r="AY12" s="9"/>
-      <c r="AZ12" s="10"/>
-      <c r="BA12" s="23"/>
-      <c r="BB12" s="23"/>
-      <c r="BC12" s="23"/>
-      <c r="BD12" s="23"/>
+      <c r="AZ12" s="9"/>
+      <c r="BA12" s="61"/>
+      <c r="BB12" s="61"/>
+      <c r="BC12" s="61"/>
+      <c r="BD12" s="61"/>
+      <c r="BE12" s="62"/>
     </row>
     <row r="13" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -2189,6 +2217,7 @@
       <c r="AZ14" s="48"/>
       <c r="BC14" s="27"/>
       <c r="BD14" s="29"/>
+      <c r="BE14" s="11"/>
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>

</xml_diff>

<commit_message>
behaviour tree fixed ish
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEABF24E-1637-4441-A0E0-982E982D4D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885D959C-39FA-493C-B16A-5E565B5D4D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -909,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9F7A41-D1C8-40CA-B4D4-A4E7F54E7CAD}">
   <dimension ref="A1:DY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="DB21" sqref="DB21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BM13" sqref="BM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2149,6 +2149,11 @@
       <c r="BB11" s="59"/>
       <c r="BC11" s="60"/>
       <c r="BF11" s="11"/>
+      <c r="BJ11" s="11"/>
+      <c r="BK11" s="11"/>
+      <c r="BL11" s="11"/>
+      <c r="BM11" s="11"/>
+      <c r="BN11" s="11"/>
     </row>
     <row r="12" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">

</xml_diff>

<commit_message>
behaviour tree fixed. behaviour tree needs search and attack sequence
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885D959C-39FA-493C-B16A-5E565B5D4D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4F8746-A173-4AE8-9728-2CB0130FAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="3530" yWindow="140" windowWidth="19640" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -910,7 +910,7 @@
   <dimension ref="A1:DY57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BM13" sqref="BM13"/>
+      <selection activeCell="BP11" sqref="BP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2154,6 +2154,7 @@
       <c r="BL11" s="11"/>
       <c r="BM11" s="11"/>
       <c r="BN11" s="11"/>
+      <c r="BO11" s="11"/>
     </row>
     <row r="12" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">

</xml_diff>

<commit_message>
broken guardSearchAttack script in behaviour tree, possible fix halfway implemented
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4F8746-A173-4AE8-9728-2CB0130FAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53147046-110F-447A-835A-0AE1FED36696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3530" yWindow="140" windowWidth="19640" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -591,8 +591,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9F7A41-D1C8-40CA-B4D4-A4E7F54E7CAD}">
   <dimension ref="A1:DY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BP11" sqref="BP11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BP15" sqref="BP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2155,6 +2153,7 @@
       <c r="BM11" s="11"/>
       <c r="BN11" s="11"/>
       <c r="BO11" s="11"/>
+      <c r="BP11" s="11"/>
     </row>
     <row r="12" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -2178,11 +2177,11 @@
       <c r="AX12" s="57"/>
       <c r="AY12" s="9"/>
       <c r="AZ12" s="9"/>
-      <c r="BA12" s="61"/>
-      <c r="BB12" s="61"/>
-      <c r="BC12" s="61"/>
-      <c r="BD12" s="61"/>
-      <c r="BE12" s="62"/>
+      <c r="BA12" s="9"/>
+      <c r="BB12" s="9"/>
+      <c r="BC12" s="9"/>
+      <c r="BD12" s="9"/>
+      <c r="BE12" s="10"/>
     </row>
     <row r="13" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
Behaviour tree COMPLETED. write-up still to do
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A118BC8C-CDCD-473F-BAD9-B7F61C1EC00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B5A4FA-24D5-4855-94AC-C7F25507F173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3530" yWindow="140" windowWidth="19640" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="3530" yWindow="140" windowWidth="22980" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -591,7 +591,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9F7A41-D1C8-40CA-B4D4-A4E7F54E7CAD}">
   <dimension ref="A1:DY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BF11" sqref="BF11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX12" sqref="AX12:BE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2155,8 +2154,8 @@
       <c r="BN11" s="11"/>
       <c r="BO11" s="11"/>
       <c r="BP11" s="11"/>
-      <c r="BQ11" s="61"/>
       <c r="BR11" s="11"/>
+      <c r="BS11" s="11"/>
     </row>
     <row r="12" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">

</xml_diff>

<commit_message>
results for objective 1 complete. Sprites designed for objective 2a
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38806F68-CD70-49DC-8C8A-72E85473B193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE61ED3-FB84-49E1-AF20-E92D72BC64F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
   <si>
     <t>Individual Project</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STILL TO-DO ATTACK CLASS </t>
+  </si>
+  <si>
+    <t>Implement GUNS FOR THE PLAYER AND GUARDS</t>
   </si>
 </sst>
 </file>
@@ -271,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +341,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -507,10 +519,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -518,9 +526,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -535,6 +541,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,7 +861,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CB10" sqref="CB10"/>
+      <selection activeCell="CG15" sqref="CG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,11 +901,9 @@
       <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="53"/>
       <c r="AK2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AW2" s="53"/>
       <c r="BO2" s="7" t="s">
         <v>48</v>
       </c>
@@ -1753,16 +1760,16 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
-      <c r="X6" s="47"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
@@ -1775,82 +1782,40 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
-      <c r="AK6" s="47"/>
-      <c r="AL6" s="47"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="40"/>
       <c r="AO6" s="2"/>
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
-      <c r="AT6" s="47"/>
-      <c r="AU6" s="47"/>
-      <c r="AV6" s="47"/>
-      <c r="AW6" s="47"/>
-      <c r="AX6" s="47"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
       <c r="AY6" s="29"/>
       <c r="AZ6" s="30"/>
-      <c r="BA6" s="47"/>
-      <c r="BB6" s="47"/>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="47"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
       <c r="BE6" s="29"/>
       <c r="BF6" s="30"/>
-      <c r="BG6" s="47"/>
-      <c r="BH6" s="47"/>
-      <c r="BI6" s="47"/>
-      <c r="BJ6" s="47"/>
-      <c r="BK6" s="47"/>
-      <c r="BL6" s="47"/>
+      <c r="BG6" s="2"/>
+      <c r="BH6" s="2"/>
+      <c r="BI6" s="2"/>
+      <c r="BJ6" s="2"/>
+      <c r="BK6" s="2"/>
+      <c r="BL6" s="2"/>
       <c r="BM6" s="29"/>
       <c r="BN6" s="30"/>
-      <c r="BO6" s="46"/>
-      <c r="BP6" s="46"/>
-      <c r="BQ6" s="46"/>
-      <c r="BR6" s="54"/>
-      <c r="BS6" s="55"/>
-      <c r="BT6" s="56"/>
-      <c r="BU6" s="46"/>
-      <c r="BV6" s="46"/>
-      <c r="BW6" s="46"/>
-      <c r="BX6" s="46"/>
-      <c r="BY6" s="46"/>
-      <c r="BZ6" s="46"/>
-      <c r="CA6" s="46"/>
-      <c r="CB6" s="46"/>
-      <c r="CC6" s="46"/>
-      <c r="CD6" s="46"/>
-      <c r="CE6" s="46"/>
-      <c r="CF6" s="46"/>
-      <c r="CG6" s="46"/>
-      <c r="CH6" s="46"/>
-      <c r="CI6" s="46"/>
-      <c r="CJ6" s="46"/>
-      <c r="CK6" s="46"/>
-      <c r="CL6" s="46"/>
-      <c r="CM6" s="46"/>
-      <c r="CN6" s="46"/>
-      <c r="CO6" s="46"/>
-      <c r="CP6" s="46"/>
-      <c r="CQ6" s="46"/>
-      <c r="CR6" s="46"/>
-      <c r="CS6" s="46"/>
-      <c r="CT6" s="46"/>
-      <c r="CU6" s="46"/>
-      <c r="CV6" s="46"/>
-      <c r="CW6" s="46"/>
-      <c r="CX6" s="46"/>
-      <c r="CY6" s="46"/>
-      <c r="CZ6" s="46"/>
-      <c r="DA6" s="46"/>
-      <c r="DB6" s="46"/>
-      <c r="DC6" s="46"/>
-      <c r="DD6" s="46"/>
-      <c r="DE6" s="46"/>
-      <c r="DF6" s="46"/>
-      <c r="DG6" s="46"/>
-      <c r="DH6" s="46"/>
+      <c r="BR6" s="50"/>
+      <c r="BS6" s="51"/>
+      <c r="BT6" s="52"/>
+      <c r="BU6" s="45"/>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
@@ -2061,18 +2026,6 @@
       <c r="E9" s="43">
         <v>45051</v>
       </c>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="AZ9" s="46"/>
-      <c r="BA9" s="46"/>
-      <c r="BB9" s="46"/>
-      <c r="BC9" s="46"/>
       <c r="BF9" s="35"/>
       <c r="BJ9" s="44"/>
       <c r="BK9" s="9"/>
@@ -2098,11 +2051,6 @@
       <c r="E10" s="43">
         <v>45037</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
       <c r="AN10" s="35"/>
       <c r="AX10" s="44"/>
       <c r="AY10" s="9"/>
@@ -2112,6 +2060,9 @@
       <c r="BC10" s="9"/>
       <c r="BD10" s="9"/>
       <c r="BE10" s="10"/>
+      <c r="BQ10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
@@ -2127,13 +2078,12 @@
       <c r="E11" s="43">
         <v>45008</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
       <c r="Z11" s="36"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="10"/>
+      <c r="BQ11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:129" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -2149,21 +2099,14 @@
       <c r="E12" s="43">
         <v>45051</v>
       </c>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
       <c r="Z12" s="35"/>
       <c r="AN12" s="35"/>
-      <c r="AZ12" s="46"/>
-      <c r="BC12" s="46"/>
-      <c r="BD12" s="46"/>
       <c r="BE12" s="44"/>
       <c r="BF12" s="10"/>
       <c r="BR12" s="44"/>
-      <c r="BS12" s="10"/>
+      <c r="BS12" s="9"/>
+      <c r="BT12" s="9"/>
+      <c r="BU12" s="10"/>
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
@@ -2310,26 +2253,12 @@
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46"/>
-      <c r="S15" s="46"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="46"/>
-      <c r="BE15" s="46"/>
-      <c r="BF15" s="46"/>
-      <c r="BG15" s="46"/>
-      <c r="BH15" s="46"/>
-      <c r="BI15" s="46"/>
-      <c r="BU15" s="57"/>
-      <c r="BV15" s="58"/>
-      <c r="BW15" s="59"/>
-      <c r="BX15" s="53"/>
-      <c r="BY15" s="53"/>
-      <c r="BZ15" s="53"/>
+      <c r="BU15" s="53"/>
+      <c r="BV15" s="54"/>
+      <c r="BW15" s="55"/>
     </row>
     <row r="16" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -2341,29 +2270,10 @@
       <c r="C16" s="27"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="46"/>
-      <c r="U16" s="46"/>
-      <c r="V16" s="46"/>
-      <c r="BH16" s="46"/>
-      <c r="BI16" s="46"/>
-      <c r="BJ16" s="46"/>
-      <c r="BK16" s="46"/>
-      <c r="BL16" s="46"/>
-      <c r="BM16" s="46"/>
-      <c r="BN16" s="46"/>
-      <c r="BW16" s="57"/>
-      <c r="BX16" s="58"/>
-      <c r="BY16" s="58"/>
-      <c r="BZ16" s="59"/>
-      <c r="CA16" s="53"/>
-      <c r="CB16" s="53"/>
-      <c r="CC16" s="53"/>
-      <c r="CD16" s="53"/>
-      <c r="CE16" s="53"/>
-      <c r="CF16" s="53"/>
-      <c r="CG16" s="53"/>
+      <c r="BW16" s="53"/>
+      <c r="BX16" s="54"/>
+      <c r="BY16" s="54"/>
+      <c r="BZ16" s="55"/>
     </row>
     <row r="17" spans="1:127" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -2375,25 +2285,8 @@
       <c r="C17" s="27"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="46"/>
-      <c r="W17" s="46"/>
-      <c r="BC17" s="46"/>
-      <c r="BD17" s="46"/>
-      <c r="BE17" s="46"/>
-      <c r="BF17" s="46"/>
-      <c r="BG17" s="46"/>
-      <c r="BH17" s="46"/>
-      <c r="BI17" s="46"/>
-      <c r="BJ17" s="46"/>
-      <c r="BK17" s="46"/>
-      <c r="BL17" s="46"/>
-      <c r="BM17" s="46"/>
-      <c r="BN17" s="46"/>
-      <c r="BO17" s="46"/>
-      <c r="BZ17" s="57"/>
-      <c r="CA17" s="59"/>
+      <c r="BZ17" s="53"/>
+      <c r="CA17" s="55"/>
     </row>
     <row r="18" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -2543,36 +2436,10 @@
       <c r="C20" s="27"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="46"/>
-      <c r="X20" s="46"/>
-      <c r="Y20" s="46"/>
-      <c r="Z20" s="46"/>
-      <c r="AA20" s="46"/>
-      <c r="AB20" s="46"/>
-      <c r="AC20" s="46"/>
-      <c r="AD20" s="46"/>
-      <c r="AE20" s="46"/>
-      <c r="BL20" s="46"/>
-      <c r="BM20" s="46"/>
-      <c r="BN20" s="46"/>
-      <c r="BO20" s="46"/>
-      <c r="BP20" s="46"/>
-      <c r="BQ20" s="46"/>
-      <c r="BR20" s="46"/>
-      <c r="BS20" s="46"/>
-      <c r="CB20" s="60"/>
-      <c r="CC20" s="61"/>
-      <c r="CD20" s="61"/>
-      <c r="CE20" s="62"/>
-      <c r="CH20" s="53"/>
-      <c r="CI20" s="53"/>
-      <c r="CJ20" s="53"/>
-      <c r="CK20" s="53"/>
-      <c r="CL20" s="53"/>
-      <c r="CM20" s="53"/>
-      <c r="CN20" s="53"/>
-      <c r="CO20" s="53"/>
+      <c r="CB20" s="56"/>
+      <c r="CC20" s="57"/>
+      <c r="CD20" s="57"/>
+      <c r="CE20" s="58"/>
     </row>
     <row r="21" spans="1:127" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -2584,21 +2451,8 @@
       <c r="C21" s="27"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="Z21" s="46"/>
-      <c r="AA21" s="46"/>
-      <c r="AB21" s="46"/>
-      <c r="AC21" s="46"/>
-      <c r="AD21" s="46"/>
-      <c r="BP21" s="46"/>
-      <c r="BQ21" s="46"/>
-      <c r="BR21" s="46"/>
-      <c r="BS21" s="46"/>
-      <c r="BT21" s="46"/>
-      <c r="CE21" s="60"/>
-      <c r="CF21" s="62"/>
-      <c r="CN21" s="53"/>
-      <c r="CO21" s="53"/>
-      <c r="CP21" s="53"/>
+      <c r="CE21" s="56"/>
+      <c r="CF21" s="58"/>
     </row>
     <row r="22" spans="1:127" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2610,23 +2464,8 @@
       <c r="C22" s="27"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="AB22" s="46"/>
-      <c r="AC22" s="46"/>
-      <c r="AD22" s="46"/>
-      <c r="AE22" s="46"/>
-      <c r="BL22" s="46"/>
-      <c r="BM22" s="46"/>
-      <c r="BN22" s="46"/>
-      <c r="BO22" s="46"/>
-      <c r="BP22" s="46"/>
-      <c r="BQ22" s="46"/>
-      <c r="BR22" s="46"/>
-      <c r="BS22" s="46"/>
-      <c r="BT22" s="46"/>
-      <c r="BU22" s="46"/>
-      <c r="BV22" s="46"/>
-      <c r="CF22" s="60"/>
-      <c r="CG22" s="62"/>
+      <c r="CF22" s="56"/>
+      <c r="CG22" s="58"/>
     </row>
     <row r="23" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
@@ -2776,21 +2615,9 @@
       <c r="C25" s="27"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="AD25" s="46"/>
-      <c r="AE25" s="46"/>
-      <c r="AF25" s="46"/>
-      <c r="AG25" s="46"/>
-      <c r="AH25" s="46"/>
-      <c r="AI25" s="46"/>
-      <c r="AJ25" s="46"/>
-      <c r="BT25" s="46"/>
-      <c r="BU25" s="46"/>
-      <c r="BV25" s="46"/>
-      <c r="BW25" s="46"/>
-      <c r="BX25" s="46"/>
-      <c r="CH25" s="63"/>
-      <c r="CI25" s="64"/>
-      <c r="CJ25" s="65"/>
+      <c r="CH25" s="59"/>
+      <c r="CI25" s="60"/>
+      <c r="CJ25" s="61"/>
     </row>
     <row r="26" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -2940,21 +2767,8 @@
       <c r="C28" s="27"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="AI28" s="46"/>
-      <c r="AJ28" s="46"/>
-      <c r="AK28" s="46"/>
-      <c r="AL28" s="46"/>
-      <c r="AM28" s="46"/>
-      <c r="AN28" s="46"/>
-      <c r="AO28" s="46"/>
-      <c r="BV28" s="46"/>
-      <c r="BW28" s="46"/>
-      <c r="BX28" s="46"/>
-      <c r="BY28" s="46"/>
-      <c r="BZ28" s="46"/>
-      <c r="CA28" s="46"/>
-      <c r="CK28" s="66"/>
-      <c r="CL28" s="67"/>
+      <c r="CK28" s="62"/>
+      <c r="CL28" s="63"/>
     </row>
     <row r="29" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
@@ -3104,14 +2918,6 @@
       <c r="C31" s="27"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="AN31" s="46"/>
-      <c r="AO31" s="46"/>
-      <c r="AP31" s="46"/>
-      <c r="AQ31" s="46"/>
-      <c r="BY31" s="46"/>
-      <c r="BZ31" s="46"/>
-      <c r="CA31" s="46"/>
-      <c r="CB31" s="46"/>
     </row>
     <row r="32" spans="1:127" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
@@ -3123,19 +2929,6 @@
       <c r="C32" s="27"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="AO32" s="46"/>
-      <c r="AP32" s="46"/>
-      <c r="AQ32" s="46"/>
-      <c r="AR32" s="46"/>
-      <c r="AS32" s="46"/>
-      <c r="BZ32" s="46"/>
-      <c r="CA32" s="46"/>
-      <c r="CB32" s="46"/>
-      <c r="CC32" s="46"/>
-      <c r="CD32" s="46"/>
-      <c r="CE32" s="46"/>
-      <c r="CF32" s="46"/>
-      <c r="CG32" s="46"/>
     </row>
     <row r="33" spans="1:127" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
@@ -3147,15 +2940,6 @@
       <c r="C33" s="27"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="AQ33" s="46"/>
-      <c r="AR33" s="46"/>
-      <c r="AS33" s="46"/>
-      <c r="AT33" s="46"/>
-      <c r="CD33" s="46"/>
-      <c r="CE33" s="46"/>
-      <c r="CF33" s="46"/>
-      <c r="CG33" s="46"/>
-      <c r="CH33" s="46"/>
     </row>
     <row r="34" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
@@ -3163,141 +2947,137 @@
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-      <c r="AQ34" s="46"/>
-      <c r="AR34" s="46"/>
-      <c r="AS34" s="46"/>
-      <c r="AT34" s="46"/>
     </row>
     <row r="35" spans="1:127" x14ac:dyDescent="0.35">
-      <c r="A35" s="48"/>
-      <c r="B35" s="49" t="s">
+      <c r="A35" s="46"/>
+      <c r="B35" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
-      <c r="T35" s="50"/>
-      <c r="U35" s="50"/>
-      <c r="V35" s="50"/>
-      <c r="W35" s="50"/>
-      <c r="X35" s="50"/>
-      <c r="Y35" s="50"/>
-      <c r="Z35" s="50"/>
-      <c r="AA35" s="50"/>
-      <c r="AB35" s="50"/>
-      <c r="AC35" s="50"/>
-      <c r="AD35" s="50"/>
-      <c r="AE35" s="50"/>
-      <c r="AF35" s="50"/>
-      <c r="AG35" s="50"/>
-      <c r="AH35" s="50"/>
-      <c r="AI35" s="50"/>
-      <c r="AJ35" s="50"/>
-      <c r="AK35" s="50"/>
-      <c r="AL35" s="50"/>
-      <c r="AM35" s="50"/>
-      <c r="AN35" s="50"/>
-      <c r="AO35" s="50"/>
-      <c r="AP35" s="50"/>
-      <c r="AQ35" s="51"/>
-      <c r="AR35" s="51"/>
-      <c r="AS35" s="51"/>
-      <c r="AT35" s="51"/>
-      <c r="AU35" s="50"/>
-      <c r="AV35" s="50"/>
-      <c r="AW35" s="50"/>
-      <c r="AX35" s="50"/>
-      <c r="AY35" s="50"/>
-      <c r="AZ35" s="50"/>
-      <c r="BA35" s="50"/>
-      <c r="BB35" s="50"/>
-      <c r="BC35" s="50"/>
-      <c r="BD35" s="50"/>
-      <c r="BE35" s="50"/>
-      <c r="BF35" s="50"/>
-      <c r="BG35" s="50"/>
-      <c r="BH35" s="50"/>
-      <c r="BI35" s="50"/>
-      <c r="BJ35" s="50"/>
-      <c r="BK35" s="50"/>
-      <c r="BL35" s="50"/>
-      <c r="BM35" s="50"/>
-      <c r="BN35" s="50"/>
-      <c r="BO35" s="50"/>
-      <c r="BP35" s="50"/>
-      <c r="BQ35" s="50"/>
-      <c r="BR35" s="50"/>
-      <c r="BS35" s="50"/>
-      <c r="BT35" s="50"/>
-      <c r="BU35" s="50"/>
-      <c r="BV35" s="50"/>
-      <c r="BW35" s="50"/>
-      <c r="BX35" s="50"/>
-      <c r="BY35" s="50"/>
-      <c r="BZ35" s="50"/>
-      <c r="CA35" s="50"/>
-      <c r="CB35" s="50"/>
-      <c r="CC35" s="50"/>
-      <c r="CD35" s="50"/>
-      <c r="CE35" s="50"/>
-      <c r="CF35" s="50"/>
-      <c r="CG35" s="50"/>
-      <c r="CH35" s="50"/>
-      <c r="CI35" s="50"/>
-      <c r="CJ35" s="50"/>
-      <c r="CK35" s="50"/>
-      <c r="CL35" s="50"/>
-      <c r="CM35" s="50"/>
-      <c r="CN35" s="50"/>
-      <c r="CO35" s="50"/>
-      <c r="CP35" s="50"/>
-      <c r="CQ35" s="50"/>
-      <c r="CR35" s="50"/>
-      <c r="CS35" s="50"/>
-      <c r="CT35" s="50"/>
-      <c r="CU35" s="50"/>
-      <c r="CV35" s="50"/>
-      <c r="CW35" s="50"/>
-      <c r="CX35" s="50"/>
-      <c r="CY35" s="50"/>
-      <c r="CZ35" s="50"/>
-      <c r="DA35" s="50"/>
-      <c r="DB35" s="50"/>
-      <c r="DC35" s="50"/>
-      <c r="DD35" s="50"/>
-      <c r="DE35" s="50"/>
-      <c r="DF35" s="50"/>
-      <c r="DG35" s="50"/>
-      <c r="DH35" s="50"/>
-      <c r="DI35" s="50"/>
-      <c r="DJ35" s="50"/>
-      <c r="DK35" s="50"/>
-      <c r="DL35" s="50"/>
-      <c r="DM35" s="50"/>
-      <c r="DN35" s="50"/>
-      <c r="DO35" s="50"/>
-      <c r="DP35" s="50"/>
-      <c r="DQ35" s="50"/>
-      <c r="DR35" s="50"/>
-      <c r="DS35" s="50"/>
-      <c r="DT35" s="50"/>
-      <c r="DU35" s="50"/>
-      <c r="DV35" s="50"/>
-      <c r="DW35" s="50"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="48"/>
+      <c r="P35" s="48"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="48"/>
+      <c r="T35" s="48"/>
+      <c r="U35" s="48"/>
+      <c r="V35" s="48"/>
+      <c r="W35" s="48"/>
+      <c r="X35" s="48"/>
+      <c r="Y35" s="48"/>
+      <c r="Z35" s="48"/>
+      <c r="AA35" s="48"/>
+      <c r="AB35" s="48"/>
+      <c r="AC35" s="48"/>
+      <c r="AD35" s="48"/>
+      <c r="AE35" s="48"/>
+      <c r="AF35" s="48"/>
+      <c r="AG35" s="48"/>
+      <c r="AH35" s="48"/>
+      <c r="AI35" s="48"/>
+      <c r="AJ35" s="48"/>
+      <c r="AK35" s="48"/>
+      <c r="AL35" s="48"/>
+      <c r="AM35" s="48"/>
+      <c r="AN35" s="48"/>
+      <c r="AO35" s="48"/>
+      <c r="AP35" s="48"/>
+      <c r="AQ35" s="48"/>
+      <c r="AR35" s="48"/>
+      <c r="AS35" s="48"/>
+      <c r="AT35" s="48"/>
+      <c r="AU35" s="48"/>
+      <c r="AV35" s="48"/>
+      <c r="AW35" s="48"/>
+      <c r="AX35" s="48"/>
+      <c r="AY35" s="48"/>
+      <c r="AZ35" s="48"/>
+      <c r="BA35" s="48"/>
+      <c r="BB35" s="48"/>
+      <c r="BC35" s="48"/>
+      <c r="BD35" s="48"/>
+      <c r="BE35" s="48"/>
+      <c r="BF35" s="48"/>
+      <c r="BG35" s="48"/>
+      <c r="BH35" s="48"/>
+      <c r="BI35" s="48"/>
+      <c r="BJ35" s="48"/>
+      <c r="BK35" s="48"/>
+      <c r="BL35" s="48"/>
+      <c r="BM35" s="48"/>
+      <c r="BN35" s="48"/>
+      <c r="BO35" s="48"/>
+      <c r="BP35" s="48"/>
+      <c r="BQ35" s="48"/>
+      <c r="BR35" s="48"/>
+      <c r="BS35" s="48"/>
+      <c r="BT35" s="48"/>
+      <c r="BU35" s="48"/>
+      <c r="BV35" s="48"/>
+      <c r="BW35" s="48"/>
+      <c r="BX35" s="48"/>
+      <c r="BY35" s="48"/>
+      <c r="BZ35" s="48"/>
+      <c r="CA35" s="48"/>
+      <c r="CB35" s="48"/>
+      <c r="CC35" s="48"/>
+      <c r="CD35" s="48"/>
+      <c r="CE35" s="48"/>
+      <c r="CF35" s="48"/>
+      <c r="CG35" s="48"/>
+      <c r="CH35" s="48"/>
+      <c r="CI35" s="48"/>
+      <c r="CJ35" s="48"/>
+      <c r="CK35" s="48"/>
+      <c r="CL35" s="48"/>
+      <c r="CM35" s="48"/>
+      <c r="CN35" s="48"/>
+      <c r="CO35" s="48"/>
+      <c r="CP35" s="48"/>
+      <c r="CQ35" s="48"/>
+      <c r="CR35" s="48"/>
+      <c r="CS35" s="48"/>
+      <c r="CT35" s="48"/>
+      <c r="CU35" s="48"/>
+      <c r="CV35" s="48"/>
+      <c r="CW35" s="48"/>
+      <c r="CX35" s="48"/>
+      <c r="CY35" s="48"/>
+      <c r="CZ35" s="48"/>
+      <c r="DA35" s="48"/>
+      <c r="DB35" s="48"/>
+      <c r="DC35" s="48"/>
+      <c r="DD35" s="48"/>
+      <c r="DE35" s="48"/>
+      <c r="DF35" s="48"/>
+      <c r="DG35" s="48"/>
+      <c r="DH35" s="48"/>
+      <c r="DI35" s="48"/>
+      <c r="DJ35" s="48"/>
+      <c r="DK35" s="48"/>
+      <c r="DL35" s="48"/>
+      <c r="DM35" s="48"/>
+      <c r="DN35" s="48"/>
+      <c r="DO35" s="48"/>
+      <c r="DP35" s="48"/>
+      <c r="DQ35" s="48"/>
+      <c r="DR35" s="48"/>
+      <c r="DS35" s="48"/>
+      <c r="DT35" s="48"/>
+      <c r="DU35" s="48"/>
+      <c r="DV35" s="48"/>
+      <c r="DW35" s="48"/>
     </row>
     <row r="36" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -3306,7 +3086,7 @@
       <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="52"/>
+      <c r="C36" s="49"/>
       <c r="D36" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
objective 2A implemented, write-up methods 2A complete, testing 2A complete
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE61ED3-FB84-49E1-AF20-E92D72BC64F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6209C584-7215-4D7A-919E-38CEB10BFD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -277,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,12 +341,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,9 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,7 +853,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CG15" sqref="CG15"/>
+      <selection activeCell="CD14" sqref="CD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1816,6 +1808,7 @@
       <c r="BS6" s="51"/>
       <c r="BT6" s="52"/>
       <c r="BU6" s="45"/>
+      <c r="BV6" s="45"/>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
@@ -2253,12 +2246,12 @@
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="64"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="BU15" s="53"/>
-      <c r="BV15" s="54"/>
-      <c r="BW15" s="55"/>
+      <c r="BV15" s="55"/>
+      <c r="BW15" s="64"/>
     </row>
     <row r="16" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -2285,6 +2278,7 @@
       <c r="C17" s="27"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
+      <c r="BV17" s="8"/>
       <c r="BZ17" s="53"/>
       <c r="CA17" s="55"/>
     </row>

</xml_diff>

<commit_message>
Objective 2b 90% implemented. gradient for bar and comments still to do.
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6209C584-7215-4D7A-919E-38CEB10BFD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4062D538-975D-4F98-A3B7-6B7D1E3E4BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="110" yWindow="130" windowWidth="22980" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +341,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -535,7 +541,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,7 +862,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CD14" sqref="CD14"/>
+      <selection activeCell="H11" sqref="H11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2247,8 +2256,12 @@
         <v>21</v>
       </c>
       <c r="C15" s="28"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="43">
+        <v>45053</v>
+      </c>
+      <c r="E15" s="43">
+        <v>45054</v>
+      </c>
       <c r="BU15" s="53"/>
       <c r="BV15" s="55"/>
       <c r="BW15" s="64"/>
@@ -2260,7 +2273,7 @@
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="BW16" s="53"/>

</xml_diff>

<commit_message>
Objective 2 completed. Requirements, methods, testing, results all done.
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4062D538-975D-4F98-A3B7-6B7D1E3E4BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC1FD61-5FAB-4BCF-8A6A-973342BD1361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="110" yWindow="130" windowWidth="22980" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,12 +341,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -542,9 +536,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,7 +856,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:M11"/>
+      <selection activeCell="CC16" sqref="CC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2273,13 +2267,17 @@
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="43">
+        <v>45055</v>
+      </c>
+      <c r="E16" s="43">
+        <v>45057</v>
+      </c>
       <c r="BW16" s="53"/>
-      <c r="BX16" s="54"/>
+      <c r="BX16" s="65"/>
       <c r="BY16" s="54"/>
-      <c r="BZ16" s="55"/>
+      <c r="BZ16" s="64"/>
     </row>
     <row r="17" spans="1:127" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -2288,12 +2286,17 @@
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="43">
+        <v>45054</v>
+      </c>
+      <c r="E17" s="43">
+        <v>45057</v>
+      </c>
       <c r="BV17" s="8"/>
-      <c r="BZ17" s="53"/>
-      <c r="CA17" s="55"/>
+      <c r="BY17" s="8"/>
+      <c r="BZ17" s="67"/>
+      <c r="CA17" s="66"/>
     </row>
     <row r="18" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>

</xml_diff>

<commit_message>
smoke bomb require ments and basic smoke bomb implemented into game
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ECC469-973E-4710-B50A-1FC347C2ADCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38CCC1E-E226-4BF7-A629-78D3CD0D16D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="110" yWindow="130" windowWidth="22980" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +341,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -539,6 +545,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9F7A41-D1C8-40CA-B4D4-A4E7F54E7CAD}">
   <dimension ref="A1:DY56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CT40" sqref="CT40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CA20" sqref="CA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2443,9 +2452,12 @@
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="43">
+        <v>45059</v>
+      </c>
       <c r="E20" s="2"/>
+      <c r="CA20" s="17"/>
       <c r="CB20" s="56"/>
       <c r="CC20" s="57"/>
       <c r="CD20" s="57"/>

</xml_diff>

<commit_message>
removed broken smoke bomb features. Basic smoke bomb implemented, mechanics part 1 completed
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38CCC1E-E226-4BF7-A629-78D3CD0D16D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09CFF81-C7B9-4025-8ADD-4DA65E650952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -534,7 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -865,7 +864,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CA20" sqref="CA20"/>
+      <selection activeCell="CP10" sqref="CP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1821,6 +1820,9 @@
       <c r="BT6" s="52"/>
       <c r="BU6" s="45"/>
       <c r="BV6" s="45"/>
+      <c r="CA6" s="45"/>
+      <c r="CB6" s="45"/>
+      <c r="CH6" s="45"/>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
@@ -2267,7 +2269,7 @@
       </c>
       <c r="BU15" s="53"/>
       <c r="BV15" s="55"/>
-      <c r="BW15" s="64"/>
+      <c r="BW15" s="63"/>
     </row>
     <row r="16" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -2284,9 +2286,9 @@
         <v>45057</v>
       </c>
       <c r="BW16" s="53"/>
-      <c r="BX16" s="65"/>
+      <c r="BX16" s="64"/>
       <c r="BY16" s="54"/>
-      <c r="BZ16" s="64"/>
+      <c r="BZ16" s="63"/>
     </row>
     <row r="17" spans="1:127" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -2304,8 +2306,8 @@
       </c>
       <c r="BV17" s="8"/>
       <c r="BY17" s="8"/>
-      <c r="BZ17" s="66"/>
-      <c r="CA17" s="64"/>
+      <c r="BZ17" s="65"/>
+      <c r="CA17" s="63"/>
     </row>
     <row r="18" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -2452,16 +2454,17 @@
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="68"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="43">
         <v>45059</v>
       </c>
       <c r="E20" s="2"/>
       <c r="CA20" s="17"/>
       <c r="CB20" s="56"/>
-      <c r="CC20" s="57"/>
-      <c r="CD20" s="57"/>
-      <c r="CE20" s="58"/>
+      <c r="CC20" s="64"/>
+      <c r="CD20" s="64"/>
+      <c r="CE20" s="63"/>
+      <c r="CH20" s="17"/>
     </row>
     <row r="21" spans="1:127" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -2474,7 +2477,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="CE21" s="56"/>
-      <c r="CF21" s="58"/>
+      <c r="CF21" s="57"/>
     </row>
     <row r="22" spans="1:127" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2487,7 +2490,8 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="CF22" s="56"/>
-      <c r="CG22" s="58"/>
+      <c r="CG22" s="57"/>
+      <c r="CH22" s="17"/>
     </row>
     <row r="23" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
@@ -2637,9 +2641,9 @@
       <c r="C25" s="27"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="CH25" s="59"/>
-      <c r="CI25" s="60"/>
-      <c r="CJ25" s="61"/>
+      <c r="CH25" s="58"/>
+      <c r="CI25" s="59"/>
+      <c r="CJ25" s="60"/>
     </row>
     <row r="26" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -2789,8 +2793,8 @@
       <c r="C28" s="27"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="CK28" s="62"/>
-      <c r="CL28" s="63"/>
+      <c r="CK28" s="61"/>
+      <c r="CL28" s="62"/>
     </row>
     <row r="29" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
@@ -3142,7 +3146,7 @@
       <c r="AU36" s="33"/>
       <c r="AV36" s="33"/>
       <c r="AW36" s="34"/>
-      <c r="BZ36" s="67"/>
+      <c r="BZ36" s="66"/>
     </row>
     <row r="37" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>

</xml_diff>

<commit_message>
Completed objective 3 fully.
Forgot to submit.
Lots of stuff.
starting new example level now.
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09CFF81-C7B9-4025-8ADD-4DA65E650952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63354A2-DA02-4354-958E-6E062C443312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="2230" yWindow="120" windowWidth="35890" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="54">
   <si>
     <t>Individual Project</t>
   </si>
@@ -188,9 +188,6 @@
     <t>June</t>
   </si>
   <si>
-    <t>IN3005 Deadline</t>
-  </si>
-  <si>
     <t xml:space="preserve">Meeting </t>
   </si>
   <si>
@@ -201,12 +198,6 @@
   </si>
   <si>
     <t>Final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STILL TO-DO ATTACK CLASS </t>
-  </si>
-  <si>
-    <t>Implement GUNS FOR THE PLAYER AND GUARDS</t>
   </si>
 </sst>
 </file>
@@ -277,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,20 +329,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -422,11 +401,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -505,7 +495,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -536,15 +525,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -864,7 +857,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CP10" sqref="CP10"/>
+      <selection activeCell="CW10" sqref="CW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -878,25 +871,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:129" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="AW1" s="41"/>
-      <c r="CB1" s="41" t="s">
+      <c r="Q1" s="40"/>
+      <c r="AW1" s="40"/>
+      <c r="CB1" s="40"/>
+      <c r="CN1" s="40"/>
+      <c r="CY1" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="DB1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="CN1" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="CY1" s="41" t="s">
+      <c r="DF1" s="40" t="s">
         <v>53</v>
-      </c>
-      <c r="DB1" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="DF1" s="41" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:129" ht="26" x14ac:dyDescent="0.6">
@@ -910,13 +899,11 @@
       <c r="BO2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="CB2" s="38"/>
-      <c r="CN2" s="45"/>
       <c r="CT2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="CY2" s="37"/>
-      <c r="DB2" s="45"/>
+      <c r="DB2" s="44"/>
       <c r="DF2" s="37"/>
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.35">
@@ -1288,19 +1275,19 @@
       </c>
     </row>
     <row r="4" spans="1:129" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="41" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1788,7 +1775,7 @@
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
-      <c r="AN6" s="40"/>
+      <c r="AN6" s="39"/>
       <c r="AO6" s="2"/>
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
@@ -1815,14 +1802,20 @@
       <c r="BL6" s="2"/>
       <c r="BM6" s="29"/>
       <c r="BN6" s="30"/>
-      <c r="BR6" s="50"/>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="52"/>
-      <c r="BU6" s="45"/>
-      <c r="BV6" s="45"/>
-      <c r="CA6" s="45"/>
-      <c r="CB6" s="45"/>
-      <c r="CH6" s="45"/>
+      <c r="BR6" s="49"/>
+      <c r="BS6" s="50"/>
+      <c r="BT6" s="50"/>
+      <c r="BU6" s="50"/>
+      <c r="BV6" s="51"/>
+      <c r="CA6" s="49"/>
+      <c r="CB6" s="51"/>
+      <c r="CH6" s="49"/>
+      <c r="CI6" s="50"/>
+      <c r="CJ6" s="51"/>
+      <c r="CO6" s="49"/>
+      <c r="CP6" s="51"/>
+      <c r="CR6" s="49"/>
+      <c r="CS6" s="51"/>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
@@ -2027,21 +2020,21 @@
         <v>14</v>
       </c>
       <c r="C9" s="28"/>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <v>45038</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="42">
         <v>45051</v>
       </c>
       <c r="BF9" s="35"/>
-      <c r="BJ9" s="44"/>
+      <c r="BJ9" s="43"/>
       <c r="BK9" s="9"/>
       <c r="BL9" s="9"/>
       <c r="BM9" s="9"/>
       <c r="BN9" s="9"/>
       <c r="BO9" s="9"/>
       <c r="BP9" s="10"/>
-      <c r="BR9" s="44"/>
+      <c r="BR9" s="43"/>
       <c r="BS9" s="10"/>
     </row>
     <row r="10" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
@@ -2052,14 +2045,14 @@
         <v>16</v>
       </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="43">
+      <c r="D10" s="42">
         <v>45020</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="42">
         <v>45037</v>
       </c>
       <c r="AN10" s="35"/>
-      <c r="AX10" s="44"/>
+      <c r="AX10" s="43"/>
       <c r="AY10" s="9"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
@@ -2067,9 +2060,6 @@
       <c r="BC10" s="9"/>
       <c r="BD10" s="9"/>
       <c r="BE10" s="10"/>
-      <c r="BQ10" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="11" spans="1:129" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
@@ -2079,18 +2069,15 @@
         <v>18</v>
       </c>
       <c r="C11" s="28"/>
-      <c r="D11" s="43">
+      <c r="D11" s="42">
         <v>45006</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="42">
         <v>45008</v>
       </c>
       <c r="Z11" s="36"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="10"/>
-      <c r="BQ11" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="12" spans="1:129" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -2100,17 +2087,17 @@
         <v>19</v>
       </c>
       <c r="C12" s="28"/>
-      <c r="D12" s="43">
+      <c r="D12" s="42">
         <v>45006</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="42">
         <v>45051</v>
       </c>
       <c r="Z12" s="35"/>
       <c r="AN12" s="35"/>
-      <c r="BE12" s="44"/>
+      <c r="BE12" s="43"/>
       <c r="BF12" s="10"/>
-      <c r="BR12" s="44"/>
+      <c r="BR12" s="43"/>
       <c r="BS12" s="9"/>
       <c r="BT12" s="9"/>
       <c r="BU12" s="10"/>
@@ -2261,15 +2248,14 @@
         <v>21</v>
       </c>
       <c r="C15" s="28"/>
-      <c r="D15" s="43">
+      <c r="D15" s="42">
         <v>45053</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <v>45054</v>
       </c>
-      <c r="BU15" s="53"/>
-      <c r="BV15" s="55"/>
-      <c r="BW15" s="63"/>
+      <c r="BU15" s="52"/>
+      <c r="BV15" s="54"/>
     </row>
     <row r="16" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -2279,16 +2265,15 @@
         <v>23</v>
       </c>
       <c r="C16" s="28"/>
-      <c r="D16" s="43">
+      <c r="D16" s="42">
         <v>45055</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="42">
         <v>45057</v>
       </c>
-      <c r="BW16" s="53"/>
-      <c r="BX16" s="64"/>
-      <c r="BY16" s="54"/>
-      <c r="BZ16" s="63"/>
+      <c r="BW16" s="52"/>
+      <c r="BX16" s="53"/>
+      <c r="BY16" s="64"/>
     </row>
     <row r="17" spans="1:127" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -2298,16 +2283,14 @@
         <v>19</v>
       </c>
       <c r="C17" s="28"/>
-      <c r="D17" s="43">
+      <c r="D17" s="42">
         <v>45054</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="42">
         <v>45057</v>
       </c>
-      <c r="BV17" s="8"/>
-      <c r="BY17" s="8"/>
-      <c r="BZ17" s="65"/>
-      <c r="CA17" s="63"/>
+      <c r="BV17" s="62"/>
+      <c r="BY17" s="62"/>
     </row>
     <row r="18" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -2454,17 +2437,33 @@
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="43">
+      <c r="C20" s="28"/>
+      <c r="D20" s="42">
         <v>45059</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="CA20" s="17"/>
-      <c r="CB20" s="56"/>
-      <c r="CC20" s="64"/>
-      <c r="CD20" s="64"/>
+      <c r="E20" s="42">
+        <v>45074</v>
+      </c>
+      <c r="CA20" s="55"/>
+      <c r="CB20" s="63"/>
+      <c r="CC20" s="63"/>
+      <c r="CD20" s="63"/>
       <c r="CE20" s="63"/>
-      <c r="CH20" s="17"/>
+      <c r="CF20" s="63"/>
+      <c r="CG20" s="63"/>
+      <c r="CH20" s="63"/>
+      <c r="CI20" s="63"/>
+      <c r="CJ20" s="63"/>
+      <c r="CK20" s="63"/>
+      <c r="CL20" s="63"/>
+      <c r="CM20" s="63"/>
+      <c r="CN20" s="63"/>
+      <c r="CO20" s="63"/>
+      <c r="CP20" s="56"/>
+      <c r="CQ20" s="65"/>
+      <c r="CR20" s="65"/>
+      <c r="CS20" s="65"/>
+      <c r="CT20" s="65"/>
     </row>
     <row r="21" spans="1:127" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -2473,11 +2472,33 @@
       <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="CE21" s="56"/>
-      <c r="CF21" s="57"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="42">
+        <v>45075</v>
+      </c>
+      <c r="E21" s="42">
+        <v>45077</v>
+      </c>
+      <c r="CA21" s="65"/>
+      <c r="CB21" s="65"/>
+      <c r="CC21" s="65"/>
+      <c r="CD21" s="65"/>
+      <c r="CE21" s="65"/>
+      <c r="CF21" s="65"/>
+      <c r="CG21" s="65"/>
+      <c r="CH21" s="66"/>
+      <c r="CI21" s="66"/>
+      <c r="CJ21" s="66"/>
+      <c r="CK21" s="66"/>
+      <c r="CL21" s="65"/>
+      <c r="CM21" s="65"/>
+      <c r="CN21" s="65"/>
+      <c r="CO21" s="65"/>
+      <c r="CP21" s="65"/>
+      <c r="CQ21" s="55"/>
+      <c r="CR21" s="63"/>
+      <c r="CS21" s="56"/>
+      <c r="CT21" s="65"/>
     </row>
     <row r="22" spans="1:127" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2486,12 +2507,33 @@
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="CF22" s="56"/>
-      <c r="CG22" s="57"/>
-      <c r="CH22" s="17"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="42">
+        <v>45076</v>
+      </c>
+      <c r="E22" s="42">
+        <v>45078</v>
+      </c>
+      <c r="CA22" s="55"/>
+      <c r="CB22" s="56"/>
+      <c r="CC22" s="65"/>
+      <c r="CD22" s="65"/>
+      <c r="CE22" s="65"/>
+      <c r="CF22" s="65"/>
+      <c r="CG22" s="65"/>
+      <c r="CH22" s="66"/>
+      <c r="CI22" s="66"/>
+      <c r="CJ22" s="66"/>
+      <c r="CK22" s="66"/>
+      <c r="CL22" s="65"/>
+      <c r="CM22" s="65"/>
+      <c r="CN22" s="65"/>
+      <c r="CO22" s="65"/>
+      <c r="CP22" s="65"/>
+      <c r="CQ22" s="65"/>
+      <c r="CR22" s="55"/>
+      <c r="CS22" s="63"/>
+      <c r="CT22" s="56"/>
     </row>
     <row r="23" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
@@ -2638,12 +2680,15 @@
       <c r="B25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="CH25" s="58"/>
-      <c r="CI25" s="59"/>
-      <c r="CJ25" s="60"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="CK25" s="66"/>
+      <c r="CL25" s="66"/>
+      <c r="CM25" s="66"/>
+      <c r="CN25" s="66"/>
+      <c r="CU25" s="57"/>
+      <c r="CV25" s="58"/>
     </row>
     <row r="26" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -2790,11 +2835,14 @@
       <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="CK28" s="61"/>
-      <c r="CL28" s="62"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="CO28" s="66"/>
+      <c r="CP28" s="66"/>
+      <c r="CQ28" s="66"/>
+      <c r="CW28" s="59"/>
+      <c r="CX28" s="60"/>
     </row>
     <row r="29" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
@@ -2975,135 +3023,135 @@
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:127" x14ac:dyDescent="0.35">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="48"/>
-      <c r="S35" s="48"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="48"/>
-      <c r="V35" s="48"/>
-      <c r="W35" s="48"/>
-      <c r="X35" s="48"/>
-      <c r="Y35" s="48"/>
-      <c r="Z35" s="48"/>
-      <c r="AA35" s="48"/>
-      <c r="AB35" s="48"/>
-      <c r="AC35" s="48"/>
-      <c r="AD35" s="48"/>
-      <c r="AE35" s="48"/>
-      <c r="AF35" s="48"/>
-      <c r="AG35" s="48"/>
-      <c r="AH35" s="48"/>
-      <c r="AI35" s="48"/>
-      <c r="AJ35" s="48"/>
-      <c r="AK35" s="48"/>
-      <c r="AL35" s="48"/>
-      <c r="AM35" s="48"/>
-      <c r="AN35" s="48"/>
-      <c r="AO35" s="48"/>
-      <c r="AP35" s="48"/>
-      <c r="AQ35" s="48"/>
-      <c r="AR35" s="48"/>
-      <c r="AS35" s="48"/>
-      <c r="AT35" s="48"/>
-      <c r="AU35" s="48"/>
-      <c r="AV35" s="48"/>
-      <c r="AW35" s="48"/>
-      <c r="AX35" s="48"/>
-      <c r="AY35" s="48"/>
-      <c r="AZ35" s="48"/>
-      <c r="BA35" s="48"/>
-      <c r="BB35" s="48"/>
-      <c r="BC35" s="48"/>
-      <c r="BD35" s="48"/>
-      <c r="BE35" s="48"/>
-      <c r="BF35" s="48"/>
-      <c r="BG35" s="48"/>
-      <c r="BH35" s="48"/>
-      <c r="BI35" s="48"/>
-      <c r="BJ35" s="48"/>
-      <c r="BK35" s="48"/>
-      <c r="BL35" s="48"/>
-      <c r="BM35" s="48"/>
-      <c r="BN35" s="48"/>
-      <c r="BO35" s="48"/>
-      <c r="BP35" s="48"/>
-      <c r="BQ35" s="48"/>
-      <c r="BR35" s="48"/>
-      <c r="BS35" s="48"/>
-      <c r="BT35" s="48"/>
-      <c r="BU35" s="48"/>
-      <c r="BV35" s="48"/>
-      <c r="BW35" s="48"/>
-      <c r="BX35" s="48"/>
-      <c r="BY35" s="48"/>
-      <c r="BZ35" s="48"/>
-      <c r="CA35" s="48"/>
-      <c r="CB35" s="48"/>
-      <c r="CC35" s="48"/>
-      <c r="CD35" s="48"/>
-      <c r="CE35" s="48"/>
-      <c r="CF35" s="48"/>
-      <c r="CG35" s="48"/>
-      <c r="CH35" s="48"/>
-      <c r="CI35" s="48"/>
-      <c r="CJ35" s="48"/>
-      <c r="CK35" s="48"/>
-      <c r="CL35" s="48"/>
-      <c r="CM35" s="48"/>
-      <c r="CN35" s="48"/>
-      <c r="CO35" s="48"/>
-      <c r="CP35" s="48"/>
-      <c r="CQ35" s="48"/>
-      <c r="CR35" s="48"/>
-      <c r="CS35" s="48"/>
-      <c r="CT35" s="48"/>
-      <c r="CU35" s="48"/>
-      <c r="CV35" s="48"/>
-      <c r="CW35" s="48"/>
-      <c r="CX35" s="48"/>
-      <c r="CY35" s="48"/>
-      <c r="CZ35" s="48"/>
-      <c r="DA35" s="48"/>
-      <c r="DB35" s="48"/>
-      <c r="DC35" s="48"/>
-      <c r="DD35" s="48"/>
-      <c r="DE35" s="48"/>
-      <c r="DF35" s="48"/>
-      <c r="DG35" s="48"/>
-      <c r="DH35" s="48"/>
-      <c r="DI35" s="48"/>
-      <c r="DJ35" s="48"/>
-      <c r="DK35" s="48"/>
-      <c r="DL35" s="48"/>
-      <c r="DM35" s="48"/>
-      <c r="DN35" s="48"/>
-      <c r="DO35" s="48"/>
-      <c r="DP35" s="48"/>
-      <c r="DQ35" s="48"/>
-      <c r="DR35" s="48"/>
-      <c r="DS35" s="48"/>
-      <c r="DT35" s="48"/>
-      <c r="DU35" s="48"/>
-      <c r="DV35" s="48"/>
-      <c r="DW35" s="48"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
+      <c r="U35" s="47"/>
+      <c r="V35" s="47"/>
+      <c r="W35" s="47"/>
+      <c r="X35" s="47"/>
+      <c r="Y35" s="47"/>
+      <c r="Z35" s="47"/>
+      <c r="AA35" s="47"/>
+      <c r="AB35" s="47"/>
+      <c r="AC35" s="47"/>
+      <c r="AD35" s="47"/>
+      <c r="AE35" s="47"/>
+      <c r="AF35" s="47"/>
+      <c r="AG35" s="47"/>
+      <c r="AH35" s="47"/>
+      <c r="AI35" s="47"/>
+      <c r="AJ35" s="47"/>
+      <c r="AK35" s="47"/>
+      <c r="AL35" s="47"/>
+      <c r="AM35" s="47"/>
+      <c r="AN35" s="47"/>
+      <c r="AO35" s="47"/>
+      <c r="AP35" s="47"/>
+      <c r="AQ35" s="47"/>
+      <c r="AR35" s="47"/>
+      <c r="AS35" s="47"/>
+      <c r="AT35" s="47"/>
+      <c r="AU35" s="47"/>
+      <c r="AV35" s="47"/>
+      <c r="AW35" s="47"/>
+      <c r="AX35" s="47"/>
+      <c r="AY35" s="47"/>
+      <c r="AZ35" s="47"/>
+      <c r="BA35" s="47"/>
+      <c r="BB35" s="47"/>
+      <c r="BC35" s="47"/>
+      <c r="BD35" s="47"/>
+      <c r="BE35" s="47"/>
+      <c r="BF35" s="47"/>
+      <c r="BG35" s="47"/>
+      <c r="BH35" s="47"/>
+      <c r="BI35" s="47"/>
+      <c r="BJ35" s="47"/>
+      <c r="BK35" s="47"/>
+      <c r="BL35" s="47"/>
+      <c r="BM35" s="47"/>
+      <c r="BN35" s="47"/>
+      <c r="BO35" s="47"/>
+      <c r="BP35" s="47"/>
+      <c r="BQ35" s="47"/>
+      <c r="BR35" s="47"/>
+      <c r="BS35" s="47"/>
+      <c r="BT35" s="47"/>
+      <c r="BU35" s="47"/>
+      <c r="BV35" s="47"/>
+      <c r="BW35" s="47"/>
+      <c r="BX35" s="47"/>
+      <c r="BY35" s="47"/>
+      <c r="BZ35" s="47"/>
+      <c r="CA35" s="47"/>
+      <c r="CB35" s="47"/>
+      <c r="CC35" s="47"/>
+      <c r="CD35" s="47"/>
+      <c r="CE35" s="47"/>
+      <c r="CF35" s="47"/>
+      <c r="CG35" s="47"/>
+      <c r="CH35" s="47"/>
+      <c r="CI35" s="47"/>
+      <c r="CJ35" s="47"/>
+      <c r="CK35" s="47"/>
+      <c r="CL35" s="47"/>
+      <c r="CM35" s="47"/>
+      <c r="CN35" s="47"/>
+      <c r="CO35" s="47"/>
+      <c r="CP35" s="47"/>
+      <c r="CQ35" s="47"/>
+      <c r="CR35" s="47"/>
+      <c r="CS35" s="47"/>
+      <c r="CT35" s="47"/>
+      <c r="CU35" s="47"/>
+      <c r="CV35" s="47"/>
+      <c r="CW35" s="47"/>
+      <c r="CX35" s="47"/>
+      <c r="CY35" s="47"/>
+      <c r="CZ35" s="47"/>
+      <c r="DA35" s="47"/>
+      <c r="DB35" s="47"/>
+      <c r="DC35" s="47"/>
+      <c r="DD35" s="47"/>
+      <c r="DE35" s="47"/>
+      <c r="DF35" s="47"/>
+      <c r="DG35" s="47"/>
+      <c r="DH35" s="47"/>
+      <c r="DI35" s="47"/>
+      <c r="DJ35" s="47"/>
+      <c r="DK35" s="47"/>
+      <c r="DL35" s="47"/>
+      <c r="DM35" s="47"/>
+      <c r="DN35" s="47"/>
+      <c r="DO35" s="47"/>
+      <c r="DP35" s="47"/>
+      <c r="DQ35" s="47"/>
+      <c r="DR35" s="47"/>
+      <c r="DS35" s="47"/>
+      <c r="DT35" s="47"/>
+      <c r="DU35" s="47"/>
+      <c r="DV35" s="47"/>
+      <c r="DW35" s="47"/>
     </row>
     <row r="36" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -3112,7 +3160,7 @@
       <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="48"/>
       <c r="D36" t="s">
         <v>45</v>
       </c>
@@ -3146,7 +3194,7 @@
       <c r="AU36" s="33"/>
       <c r="AV36" s="33"/>
       <c r="AW36" s="34"/>
-      <c r="BZ36" s="66"/>
+      <c r="BZ36" s="61"/>
     </row>
     <row r="37" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>

</xml_diff>

<commit_message>
final report half written up
</commit_message>
<xml_diff>
--- a/Gantt Charts/Gantt Chart Updated.xlsx
+++ b/Gantt Charts/Gantt Chart Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T4YY4\Documents\GitHub\Individual Project\individualProject\Gantt Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63354A2-DA02-4354-958E-6E062C443312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28175253-9807-49E1-9DA3-CC48C1E8EEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2230" yWindow="120" windowWidth="35890" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
+    <workbookView xWindow="17640" yWindow="180" windowWidth="20410" windowHeight="20480" xr2:uid="{86D6CAE1-6D93-47A6-A03C-9E8F185825C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="53">
   <si>
     <t>Individual Project</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Other Coursework</t>
-  </si>
-  <si>
-    <t>Code</t>
   </si>
   <si>
     <t>Final</t>
@@ -416,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -474,9 +471,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -526,20 +520,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,7 +848,7 @@
   <dimension ref="A1:DY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CW10" sqref="CW10"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -871,21 +862,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:129" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="AW1" s="40"/>
-      <c r="CB1" s="40"/>
-      <c r="CN1" s="40"/>
-      <c r="CY1" s="40" t="s">
+      <c r="Q1" s="39"/>
+      <c r="AW1" s="39"/>
+      <c r="CB1" s="39"/>
+      <c r="CN1" s="39"/>
+      <c r="CY1" s="39"/>
+      <c r="DB1" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="DF1" s="39" t="s">
         <v>52</v>
-      </c>
-      <c r="DB1" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="DF1" s="40" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:129" ht="26" x14ac:dyDescent="0.6">
@@ -902,9 +891,9 @@
       <c r="CT2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="CY2" s="37"/>
-      <c r="DB2" s="44"/>
-      <c r="DF2" s="37"/>
+      <c r="CY2" s="66"/>
+      <c r="DB2" s="43"/>
+      <c r="DF2" s="36"/>
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.35">
       <c r="F3">
@@ -1275,19 +1264,19 @@
       </c>
     </row>
     <row r="4" spans="1:129" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="40" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1764,9 +1753,9 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="31"/>
-      <c r="AE6" s="30"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="29"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
@@ -1775,7 +1764,7 @@
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
-      <c r="AN6" s="39"/>
+      <c r="AN6" s="38"/>
       <c r="AO6" s="2"/>
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
@@ -1786,36 +1775,43 @@
       <c r="AV6" s="2"/>
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
-      <c r="AY6" s="29"/>
-      <c r="AZ6" s="30"/>
+      <c r="AY6" s="28"/>
+      <c r="AZ6" s="29"/>
       <c r="BA6" s="2"/>
       <c r="BB6" s="2"/>
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
-      <c r="BE6" s="29"/>
-      <c r="BF6" s="30"/>
+      <c r="BE6" s="28"/>
+      <c r="BF6" s="29"/>
       <c r="BG6" s="2"/>
       <c r="BH6" s="2"/>
       <c r="BI6" s="2"/>
       <c r="BJ6" s="2"/>
       <c r="BK6" s="2"/>
       <c r="BL6" s="2"/>
-      <c r="BM6" s="29"/>
-      <c r="BN6" s="30"/>
-      <c r="BR6" s="49"/>
-      <c r="BS6" s="50"/>
-      <c r="BT6" s="50"/>
-      <c r="BU6" s="50"/>
-      <c r="BV6" s="51"/>
-      <c r="CA6" s="49"/>
-      <c r="CB6" s="51"/>
-      <c r="CH6" s="49"/>
-      <c r="CI6" s="50"/>
-      <c r="CJ6" s="51"/>
-      <c r="CO6" s="49"/>
-      <c r="CP6" s="51"/>
-      <c r="CR6" s="49"/>
-      <c r="CS6" s="51"/>
+      <c r="BM6" s="28"/>
+      <c r="BN6" s="29"/>
+      <c r="BR6" s="48"/>
+      <c r="BS6" s="49"/>
+      <c r="BT6" s="49"/>
+      <c r="BU6" s="49"/>
+      <c r="BV6" s="50"/>
+      <c r="CA6" s="48"/>
+      <c r="CB6" s="50"/>
+      <c r="CH6" s="48"/>
+      <c r="CI6" s="49"/>
+      <c r="CJ6" s="50"/>
+      <c r="CO6" s="48"/>
+      <c r="CP6" s="50"/>
+      <c r="CR6" s="48"/>
+      <c r="CS6" s="50"/>
+      <c r="CZ6" s="48"/>
+      <c r="DA6" s="49"/>
+      <c r="DB6" s="49"/>
+      <c r="DC6" s="49"/>
+      <c r="DD6" s="49"/>
+      <c r="DE6" s="49"/>
+      <c r="DF6" s="50"/>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
@@ -2019,22 +2015,22 @@
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="42">
+      <c r="C9" s="27"/>
+      <c r="D9" s="41">
         <v>45038</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="41">
         <v>45051</v>
       </c>
-      <c r="BF9" s="35"/>
-      <c r="BJ9" s="43"/>
+      <c r="BF9" s="34"/>
+      <c r="BJ9" s="42"/>
       <c r="BK9" s="9"/>
       <c r="BL9" s="9"/>
       <c r="BM9" s="9"/>
       <c r="BN9" s="9"/>
       <c r="BO9" s="9"/>
       <c r="BP9" s="10"/>
-      <c r="BR9" s="43"/>
+      <c r="BR9" s="42"/>
       <c r="BS9" s="10"/>
     </row>
     <row r="10" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
@@ -2044,15 +2040,15 @@
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="42">
+      <c r="C10" s="27"/>
+      <c r="D10" s="41">
         <v>45020</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="41">
         <v>45037</v>
       </c>
-      <c r="AN10" s="35"/>
-      <c r="AX10" s="43"/>
+      <c r="AN10" s="34"/>
+      <c r="AX10" s="42"/>
       <c r="AY10" s="9"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9"/>
@@ -2068,14 +2064,14 @@
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="42">
+      <c r="C11" s="27"/>
+      <c r="D11" s="41">
         <v>45006</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="41">
         <v>45008</v>
       </c>
-      <c r="Z11" s="36"/>
+      <c r="Z11" s="35"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="10"/>
     </row>
@@ -2086,18 +2082,18 @@
       <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="42">
+      <c r="C12" s="27"/>
+      <c r="D12" s="41">
         <v>45006</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="41">
         <v>45051</v>
       </c>
-      <c r="Z12" s="35"/>
-      <c r="AN12" s="35"/>
-      <c r="BE12" s="43"/>
+      <c r="Z12" s="34"/>
+      <c r="AN12" s="34"/>
+      <c r="BE12" s="42"/>
       <c r="BF12" s="10"/>
-      <c r="BR12" s="43"/>
+      <c r="BR12" s="42"/>
       <c r="BS12" s="9"/>
       <c r="BT12" s="9"/>
       <c r="BU12" s="10"/>
@@ -2247,15 +2243,15 @@
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="42">
+      <c r="C15" s="27"/>
+      <c r="D15" s="41">
         <v>45053</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="41">
         <v>45054</v>
       </c>
-      <c r="BU15" s="52"/>
-      <c r="BV15" s="54"/>
+      <c r="BU15" s="51"/>
+      <c r="BV15" s="53"/>
     </row>
     <row r="16" spans="1:129" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -2264,16 +2260,16 @@
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="42">
+      <c r="C16" s="27"/>
+      <c r="D16" s="41">
         <v>45055</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="41">
         <v>45057</v>
       </c>
-      <c r="BW16" s="52"/>
-      <c r="BX16" s="53"/>
-      <c r="BY16" s="64"/>
+      <c r="BW16" s="51"/>
+      <c r="BX16" s="52"/>
+      <c r="BY16" s="61"/>
     </row>
     <row r="17" spans="1:127" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -2282,15 +2278,15 @@
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="42">
+      <c r="C17" s="27"/>
+      <c r="D17" s="41">
         <v>45054</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="41">
         <v>45057</v>
       </c>
-      <c r="BV17" s="62"/>
-      <c r="BY17" s="62"/>
+      <c r="BV17" s="59"/>
+      <c r="BY17" s="59"/>
     </row>
     <row r="18" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -2437,33 +2433,29 @@
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="42">
+      <c r="C20" s="27"/>
+      <c r="D20" s="41">
         <v>45059</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="41">
         <v>45074</v>
       </c>
-      <c r="CA20" s="55"/>
-      <c r="CB20" s="63"/>
-      <c r="CC20" s="63"/>
-      <c r="CD20" s="63"/>
-      <c r="CE20" s="63"/>
-      <c r="CF20" s="63"/>
-      <c r="CG20" s="63"/>
-      <c r="CH20" s="63"/>
-      <c r="CI20" s="63"/>
-      <c r="CJ20" s="63"/>
-      <c r="CK20" s="63"/>
-      <c r="CL20" s="63"/>
-      <c r="CM20" s="63"/>
-      <c r="CN20" s="63"/>
-      <c r="CO20" s="63"/>
-      <c r="CP20" s="56"/>
-      <c r="CQ20" s="65"/>
-      <c r="CR20" s="65"/>
-      <c r="CS20" s="65"/>
-      <c r="CT20" s="65"/>
+      <c r="CA20" s="54"/>
+      <c r="CB20" s="60"/>
+      <c r="CC20" s="60"/>
+      <c r="CD20" s="60"/>
+      <c r="CE20" s="60"/>
+      <c r="CF20" s="60"/>
+      <c r="CG20" s="60"/>
+      <c r="CH20" s="60"/>
+      <c r="CI20" s="60"/>
+      <c r="CJ20" s="60"/>
+      <c r="CK20" s="60"/>
+      <c r="CL20" s="60"/>
+      <c r="CM20" s="60"/>
+      <c r="CN20" s="60"/>
+      <c r="CO20" s="60"/>
+      <c r="CP20" s="55"/>
     </row>
     <row r="21" spans="1:127" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -2472,33 +2464,16 @@
       <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="42">
+      <c r="C21" s="27"/>
+      <c r="D21" s="41">
         <v>45075</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="41">
         <v>45077</v>
       </c>
-      <c r="CA21" s="65"/>
-      <c r="CB21" s="65"/>
-      <c r="CC21" s="65"/>
-      <c r="CD21" s="65"/>
-      <c r="CE21" s="65"/>
-      <c r="CF21" s="65"/>
-      <c r="CG21" s="65"/>
-      <c r="CH21" s="66"/>
-      <c r="CI21" s="66"/>
-      <c r="CJ21" s="66"/>
-      <c r="CK21" s="66"/>
-      <c r="CL21" s="65"/>
-      <c r="CM21" s="65"/>
-      <c r="CN21" s="65"/>
-      <c r="CO21" s="65"/>
-      <c r="CP21" s="65"/>
-      <c r="CQ21" s="55"/>
-      <c r="CR21" s="63"/>
-      <c r="CS21" s="56"/>
-      <c r="CT21" s="65"/>
+      <c r="CQ21" s="54"/>
+      <c r="CR21" s="60"/>
+      <c r="CS21" s="55"/>
     </row>
     <row r="22" spans="1:127" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2507,33 +2482,18 @@
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="42">
+      <c r="C22" s="27"/>
+      <c r="D22" s="41">
         <v>45076</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="41">
         <v>45078</v>
       </c>
-      <c r="CA22" s="55"/>
-      <c r="CB22" s="56"/>
-      <c r="CC22" s="65"/>
-      <c r="CD22" s="65"/>
-      <c r="CE22" s="65"/>
-      <c r="CF22" s="65"/>
-      <c r="CG22" s="65"/>
-      <c r="CH22" s="66"/>
-      <c r="CI22" s="66"/>
-      <c r="CJ22" s="66"/>
-      <c r="CK22" s="66"/>
-      <c r="CL22" s="65"/>
-      <c r="CM22" s="65"/>
-      <c r="CN22" s="65"/>
-      <c r="CO22" s="65"/>
-      <c r="CP22" s="65"/>
-      <c r="CQ22" s="65"/>
-      <c r="CR22" s="55"/>
-      <c r="CS22" s="63"/>
-      <c r="CT22" s="56"/>
+      <c r="CA22" s="54"/>
+      <c r="CB22" s="55"/>
+      <c r="CR22" s="54"/>
+      <c r="CS22" s="60"/>
+      <c r="CT22" s="55"/>
     </row>
     <row r="23" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
@@ -2680,15 +2640,18 @@
       <c r="B25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="67"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="CK25" s="66"/>
-      <c r="CL25" s="66"/>
-      <c r="CM25" s="66"/>
-      <c r="CN25" s="66"/>
-      <c r="CU25" s="57"/>
-      <c r="CV25" s="58"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="41">
+        <v>45079</v>
+      </c>
+      <c r="E25" s="41">
+        <v>45083</v>
+      </c>
+      <c r="CU25" s="56"/>
+      <c r="CV25" s="63"/>
+      <c r="CW25" s="63"/>
+      <c r="CX25" s="63"/>
+      <c r="CY25" s="57"/>
     </row>
     <row r="26" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -2835,14 +2798,12 @@
       <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="CO28" s="66"/>
-      <c r="CP28" s="66"/>
-      <c r="CQ28" s="66"/>
-      <c r="CW28" s="59"/>
-      <c r="CX28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="CW28" s="64"/>
+      <c r="CX28" s="64"/>
+      <c r="CY28" s="65"/>
     </row>
     <row r="29" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
@@ -2989,7 +2950,7 @@
       <c r="B31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="27"/>
+      <c r="C31" s="62"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
@@ -3000,7 +2961,7 @@
       <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="62"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
@@ -3011,7 +2972,7 @@
       <c r="B33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="27"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
@@ -3023,135 +2984,135 @@
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:127" x14ac:dyDescent="0.35">
-      <c r="A35" s="45"/>
-      <c r="B35" s="46" t="s">
+      <c r="A35" s="44"/>
+      <c r="B35" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="47"/>
-      <c r="Q35" s="47"/>
-      <c r="R35" s="47"/>
-      <c r="S35" s="47"/>
-      <c r="T35" s="47"/>
-      <c r="U35" s="47"/>
-      <c r="V35" s="47"/>
-      <c r="W35" s="47"/>
-      <c r="X35" s="47"/>
-      <c r="Y35" s="47"/>
-      <c r="Z35" s="47"/>
-      <c r="AA35" s="47"/>
-      <c r="AB35" s="47"/>
-      <c r="AC35" s="47"/>
-      <c r="AD35" s="47"/>
-      <c r="AE35" s="47"/>
-      <c r="AF35" s="47"/>
-      <c r="AG35" s="47"/>
-      <c r="AH35" s="47"/>
-      <c r="AI35" s="47"/>
-      <c r="AJ35" s="47"/>
-      <c r="AK35" s="47"/>
-      <c r="AL35" s="47"/>
-      <c r="AM35" s="47"/>
-      <c r="AN35" s="47"/>
-      <c r="AO35" s="47"/>
-      <c r="AP35" s="47"/>
-      <c r="AQ35" s="47"/>
-      <c r="AR35" s="47"/>
-      <c r="AS35" s="47"/>
-      <c r="AT35" s="47"/>
-      <c r="AU35" s="47"/>
-      <c r="AV35" s="47"/>
-      <c r="AW35" s="47"/>
-      <c r="AX35" s="47"/>
-      <c r="AY35" s="47"/>
-      <c r="AZ35" s="47"/>
-      <c r="BA35" s="47"/>
-      <c r="BB35" s="47"/>
-      <c r="BC35" s="47"/>
-      <c r="BD35" s="47"/>
-      <c r="BE35" s="47"/>
-      <c r="BF35" s="47"/>
-      <c r="BG35" s="47"/>
-      <c r="BH35" s="47"/>
-      <c r="BI35" s="47"/>
-      <c r="BJ35" s="47"/>
-      <c r="BK35" s="47"/>
-      <c r="BL35" s="47"/>
-      <c r="BM35" s="47"/>
-      <c r="BN35" s="47"/>
-      <c r="BO35" s="47"/>
-      <c r="BP35" s="47"/>
-      <c r="BQ35" s="47"/>
-      <c r="BR35" s="47"/>
-      <c r="BS35" s="47"/>
-      <c r="BT35" s="47"/>
-      <c r="BU35" s="47"/>
-      <c r="BV35" s="47"/>
-      <c r="BW35" s="47"/>
-      <c r="BX35" s="47"/>
-      <c r="BY35" s="47"/>
-      <c r="BZ35" s="47"/>
-      <c r="CA35" s="47"/>
-      <c r="CB35" s="47"/>
-      <c r="CC35" s="47"/>
-      <c r="CD35" s="47"/>
-      <c r="CE35" s="47"/>
-      <c r="CF35" s="47"/>
-      <c r="CG35" s="47"/>
-      <c r="CH35" s="47"/>
-      <c r="CI35" s="47"/>
-      <c r="CJ35" s="47"/>
-      <c r="CK35" s="47"/>
-      <c r="CL35" s="47"/>
-      <c r="CM35" s="47"/>
-      <c r="CN35" s="47"/>
-      <c r="CO35" s="47"/>
-      <c r="CP35" s="47"/>
-      <c r="CQ35" s="47"/>
-      <c r="CR35" s="47"/>
-      <c r="CS35" s="47"/>
-      <c r="CT35" s="47"/>
-      <c r="CU35" s="47"/>
-      <c r="CV35" s="47"/>
-      <c r="CW35" s="47"/>
-      <c r="CX35" s="47"/>
-      <c r="CY35" s="47"/>
-      <c r="CZ35" s="47"/>
-      <c r="DA35" s="47"/>
-      <c r="DB35" s="47"/>
-      <c r="DC35" s="47"/>
-      <c r="DD35" s="47"/>
-      <c r="DE35" s="47"/>
-      <c r="DF35" s="47"/>
-      <c r="DG35" s="47"/>
-      <c r="DH35" s="47"/>
-      <c r="DI35" s="47"/>
-      <c r="DJ35" s="47"/>
-      <c r="DK35" s="47"/>
-      <c r="DL35" s="47"/>
-      <c r="DM35" s="47"/>
-      <c r="DN35" s="47"/>
-      <c r="DO35" s="47"/>
-      <c r="DP35" s="47"/>
-      <c r="DQ35" s="47"/>
-      <c r="DR35" s="47"/>
-      <c r="DS35" s="47"/>
-      <c r="DT35" s="47"/>
-      <c r="DU35" s="47"/>
-      <c r="DV35" s="47"/>
-      <c r="DW35" s="47"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="46"/>
+      <c r="S35" s="46"/>
+      <c r="T35" s="46"/>
+      <c r="U35" s="46"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="46"/>
+      <c r="Z35" s="46"/>
+      <c r="AA35" s="46"/>
+      <c r="AB35" s="46"/>
+      <c r="AC35" s="46"/>
+      <c r="AD35" s="46"/>
+      <c r="AE35" s="46"/>
+      <c r="AF35" s="46"/>
+      <c r="AG35" s="46"/>
+      <c r="AH35" s="46"/>
+      <c r="AI35" s="46"/>
+      <c r="AJ35" s="46"/>
+      <c r="AK35" s="46"/>
+      <c r="AL35" s="46"/>
+      <c r="AM35" s="46"/>
+      <c r="AN35" s="46"/>
+      <c r="AO35" s="46"/>
+      <c r="AP35" s="46"/>
+      <c r="AQ35" s="46"/>
+      <c r="AR35" s="46"/>
+      <c r="AS35" s="46"/>
+      <c r="AT35" s="46"/>
+      <c r="AU35" s="46"/>
+      <c r="AV35" s="46"/>
+      <c r="AW35" s="46"/>
+      <c r="AX35" s="46"/>
+      <c r="AY35" s="46"/>
+      <c r="AZ35" s="46"/>
+      <c r="BA35" s="46"/>
+      <c r="BB35" s="46"/>
+      <c r="BC35" s="46"/>
+      <c r="BD35" s="46"/>
+      <c r="BE35" s="46"/>
+      <c r="BF35" s="46"/>
+      <c r="BG35" s="46"/>
+      <c r="BH35" s="46"/>
+      <c r="BI35" s="46"/>
+      <c r="BJ35" s="46"/>
+      <c r="BK35" s="46"/>
+      <c r="BL35" s="46"/>
+      <c r="BM35" s="46"/>
+      <c r="BN35" s="46"/>
+      <c r="BO35" s="46"/>
+      <c r="BP35" s="46"/>
+      <c r="BQ35" s="46"/>
+      <c r="BR35" s="46"/>
+      <c r="BS35" s="46"/>
+      <c r="BT35" s="46"/>
+      <c r="BU35" s="46"/>
+      <c r="BV35" s="46"/>
+      <c r="BW35" s="46"/>
+      <c r="BX35" s="46"/>
+      <c r="BY35" s="46"/>
+      <c r="BZ35" s="46"/>
+      <c r="CA35" s="46"/>
+      <c r="CB35" s="46"/>
+      <c r="CC35" s="46"/>
+      <c r="CD35" s="46"/>
+      <c r="CE35" s="46"/>
+      <c r="CF35" s="46"/>
+      <c r="CG35" s="46"/>
+      <c r="CH35" s="46"/>
+      <c r="CI35" s="46"/>
+      <c r="CJ35" s="46"/>
+      <c r="CK35" s="46"/>
+      <c r="CL35" s="46"/>
+      <c r="CM35" s="46"/>
+      <c r="CN35" s="46"/>
+      <c r="CO35" s="46"/>
+      <c r="CP35" s="46"/>
+      <c r="CQ35" s="46"/>
+      <c r="CR35" s="46"/>
+      <c r="CS35" s="46"/>
+      <c r="CT35" s="46"/>
+      <c r="CU35" s="46"/>
+      <c r="CV35" s="46"/>
+      <c r="CW35" s="46"/>
+      <c r="CX35" s="46"/>
+      <c r="CY35" s="46"/>
+      <c r="CZ35" s="46"/>
+      <c r="DA35" s="46"/>
+      <c r="DB35" s="46"/>
+      <c r="DC35" s="46"/>
+      <c r="DD35" s="46"/>
+      <c r="DE35" s="46"/>
+      <c r="DF35" s="46"/>
+      <c r="DG35" s="46"/>
+      <c r="DH35" s="46"/>
+      <c r="DI35" s="46"/>
+      <c r="DJ35" s="46"/>
+      <c r="DK35" s="46"/>
+      <c r="DL35" s="46"/>
+      <c r="DM35" s="46"/>
+      <c r="DN35" s="46"/>
+      <c r="DO35" s="46"/>
+      <c r="DP35" s="46"/>
+      <c r="DQ35" s="46"/>
+      <c r="DR35" s="46"/>
+      <c r="DS35" s="46"/>
+      <c r="DT35" s="46"/>
+      <c r="DU35" s="46"/>
+      <c r="DV35" s="46"/>
+      <c r="DW35" s="46"/>
     </row>
     <row r="36" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -3160,41 +3121,41 @@
       <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="48"/>
+      <c r="C36" s="47"/>
       <c r="D36" t="s">
         <v>45</v>
       </c>
       <c r="E36" t="s">
         <v>45</v>
       </c>
-      <c r="K36" s="32"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="34"/>
-      <c r="AC36" s="32"/>
-      <c r="AD36" s="33"/>
-      <c r="AE36" s="33"/>
-      <c r="AF36" s="33"/>
-      <c r="AG36" s="33"/>
-      <c r="AH36" s="33"/>
-      <c r="AI36" s="33"/>
-      <c r="AJ36" s="33"/>
-      <c r="AK36" s="33"/>
-      <c r="AL36" s="33"/>
-      <c r="AM36" s="34"/>
-      <c r="AO36" s="32"/>
-      <c r="AP36" s="33"/>
-      <c r="AQ36" s="33"/>
-      <c r="AR36" s="33"/>
-      <c r="AS36" s="33"/>
-      <c r="AT36" s="33"/>
-      <c r="AU36" s="33"/>
-      <c r="AV36" s="33"/>
-      <c r="AW36" s="34"/>
-      <c r="BZ36" s="61"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="33"/>
+      <c r="AC36" s="31"/>
+      <c r="AD36" s="32"/>
+      <c r="AE36" s="32"/>
+      <c r="AF36" s="32"/>
+      <c r="AG36" s="32"/>
+      <c r="AH36" s="32"/>
+      <c r="AI36" s="32"/>
+      <c r="AJ36" s="32"/>
+      <c r="AK36" s="32"/>
+      <c r="AL36" s="32"/>
+      <c r="AM36" s="33"/>
+      <c r="AO36" s="31"/>
+      <c r="AP36" s="32"/>
+      <c r="AQ36" s="32"/>
+      <c r="AR36" s="32"/>
+      <c r="AS36" s="32"/>
+      <c r="AT36" s="32"/>
+      <c r="AU36" s="32"/>
+      <c r="AV36" s="32"/>
+      <c r="AW36" s="33"/>
+      <c r="BZ36" s="58"/>
     </row>
     <row r="37" spans="1:127" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>

</xml_diff>